<commit_message>
BIS-1985: Added xls import/export + tests
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t xml:space="preserve">SAMPLE_TYPE</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ontology Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type Group</t>
   </si>
   <si>
     <t xml:space="preserve">ENTRY</t>
@@ -154,6 +157,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -259,17 +263,17 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -297,25 +301,28 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -329,46 +336,46 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>7</v>
@@ -382,42 +389,42 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -425,44 +432,44 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -470,42 +477,42 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>

</xml_diff>